<commit_message>
wrong spelling - ganttChart
</commit_message>
<xml_diff>
--- a/Report3_GUI_Testing/Gantt/GrantChart.xlsx
+++ b/Report3_GUI_Testing/Gantt/GrantChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenbaolong/Desktop/Không phải nháp/CinemaManagementSystem/Report3_GUI_Testing/Gantt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C89E97D-0469-8E4E-8188-8B15A1678B80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6FDF6D-3E4B-AC46-BA33-78C79A84A2F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1464,9 +1464,9 @@
   </sheetPr>
   <dimension ref="A1:CR28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="U1" zoomScale="125" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CE42" sqref="CE42"/>
+      <selection pane="bottomLeft" activeCell="BD13" sqref="BD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4477,7 +4477,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:I7 H8:W8 H9:AJ9 H12:AV12 BE12:CB12 H21:BK21 H24:BR24 H25:CF25 L7:CM7 Z8:CM8 AN9:AV9 H10:CM11 CJ12:CM12 H13:CM20 H22:CM23 H26:CM28 BQ21:CM21 BZ24:CM24 CK25:CM25 AX9:CM9">
+  <conditionalFormatting sqref="H7:I7 H8:W8 H9:AJ9 H12:AV12 BE12:CB12 H21:BK21 H24:BR24 H25:CF25 L7:CM7 Z8:CM8 AN9:AV9 CJ12:CM12 H13:CM20 H22:CM23 H26:CM28 BQ21:CM21 BZ24:CM24 CK25:CM25 AX9:CM9 H10:CM11">
     <cfRule type="expression" dxfId="15" priority="28">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -4485,7 +4485,7 @@
       <formula>AND(task_end&gt;=H$5,task_start&lt;H$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:I7 L7:BK7 H8:W8 Z8:BK8 H9:AJ9 AN9:AV9 BL24:BR24 BL25:CF25 H5:CR6 BL7:CM11 CJ12:CM12 BL13:CM20 BL22:CM23 BL26:CM28 BQ21:CM21 BZ24:CM24 CK25:CM25 AX9:BK9 H10:BK11 H13:BK28 H12:AV12 BE12:CB12">
+  <conditionalFormatting sqref="H7:I7 L7:BK7 H8:W8 Z8:BK8 H9:AJ9 AN9:AV9 BL24:BR24 BL25:CF25 H5:CR6 BL7:CM11 CJ12:CM12 BL13:CM20 BL22:CM23 BL26:CM28 BQ21:CM21 BZ24:CM24 CK25:CM25 AX9:BK9 H13:BK28 H12:AV12 BE12:CB12 H10:BK11">
     <cfRule type="expression" dxfId="13" priority="30">
       <formula>AND(today&gt;=H$5,today&lt;H$5+1)</formula>
     </cfRule>

</xml_diff>